<commit_message>
schedule page is modified with an initial draft
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\UO Teaching\EDLD 654\c4-ml-fall-2021\website-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518F3B61-5432-4042-AC28-3943370D0007}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D91738-6735-433A-A17B-9D236750A40A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>week</t>
   </si>
@@ -36,9 +36,6 @@
     <t>theme</t>
   </si>
   <si>
-    <t>Introduction</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -72,58 +69,76 @@
     <t>assignments/#final-project</t>
   </si>
   <si>
-    <t>Data types</t>
-  </si>
-  <si>
-    <t>Weekly schedule of topics and an overview of the course requirements. We will also have an intro to data types.</t>
-  </si>
-  <si>
-    <t>We will finish up on discussing the four basic data types in depth and how coercion occurs. We will also discuss attributes, introduce lists, and discuss subsetting for lists versus atomic vectors.</t>
-  </si>
-  <si>
     <t>w1p1</t>
   </si>
   <si>
-    <t>w1p2</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>3.1;</t>
-  </si>
-  <si>
-    <t>4;</t>
-  </si>
-  <si>
-    <t>6; 3.4;</t>
-  </si>
-  <si>
-    <t>#pages=210; resampling.html;</t>
-  </si>
-  <si>
-    <t>esl; feat;</t>
-  </si>
-  <si>
-    <t>isl;</t>
-  </si>
-  <si>
-    <t>mml;</t>
-  </si>
-  <si>
-    <t>#pages=77;</t>
-  </si>
-  <si>
-    <t>#pages=136;</t>
-  </si>
-  <si>
-    <t>hands; hands;</t>
-  </si>
-  <si>
-    <t>process.html#prerequisites; linear-regression.html#multi-lm;</t>
-  </si>
-  <si>
-    <t>2.1; 4.3;</t>
+    <t>Warm-up I: Linear Algebra</t>
+  </si>
+  <si>
+    <t>Warm-up II: Optimization</t>
+  </si>
+  <si>
+    <t>A brief overview of some linear algebra concepts will be introduced using R to develop some terminology.</t>
+  </si>
+  <si>
+    <t>A brief overview of some calculus and optimization will be introduced using R.</t>
+  </si>
+  <si>
+    <t>Evaluation Metrics</t>
+  </si>
+  <si>
+    <t>Overfitting and Resampling Techniques</t>
+  </si>
+  <si>
+    <t>Introduction to Machine Learning</t>
+  </si>
+  <si>
+    <t>mml2</t>
+  </si>
+  <si>
+    <t>#pages=1</t>
+  </si>
+  <si>
+    <t>#pages=27</t>
+  </si>
+  <si>
+    <t>Several measures to evaluate the performance of a set of predictions will be introduced in the context of predicting a continuous outcome, a binary outcome, and a multi-class outcome.</t>
+  </si>
+  <si>
+    <t>hands; apm</t>
+  </si>
+  <si>
+    <t>process.html;</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>hands;isl</t>
+  </si>
+  <si>
+    <t>intro.html;#pages=27</t>
+  </si>
+  <si>
+    <t>apm;apm;scikit</t>
+  </si>
+  <si>
+    <t>Ch. 3</t>
+  </si>
+  <si>
+    <t>Ch. 4</t>
+  </si>
+  <si>
+    <t>Ch. 5.1;Ch. 11.1;'""</t>
+  </si>
+  <si>
+    <t>Ch. 2; Ch. 4</t>
+  </si>
+  <si>
+    <t>Ch. 1; Ch. 2.1-2.2</t>
   </si>
 </sst>
 </file>
@@ -493,11 +508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M3" sqref="M3"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -510,9 +525,10 @@
     <col min="7" max="7" width="21.19921875" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.296875" style="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="11" width="10.796875" style="1"/>
+    <col min="10" max="10" width="10.796875" style="1"/>
+    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="34.19921875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.8984375" style="1" customWidth="1"/>
     <col min="14" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
@@ -527,34 +543,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
@@ -562,40 +578,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>44284</v>
+        <v>44466</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -603,122 +619,144 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>44286</v>
+        <v>44468</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>44284</v>
+        <v>44473</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>44286</v>
+        <v>44475</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44480</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notes on linear algebra added
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\UO Teaching\EDLD 654\c4-ml-fall-2021\website-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D91738-6735-433A-A17B-9D236750A40A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5D6F04-E3A0-498B-A168-4DC22E982C02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>week</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Ch. 1; Ch. 2.1-2.2</t>
+  </si>
+  <si>
+    <t>warm-up-1</t>
   </si>
 </sst>
 </file>
@@ -510,9 +513,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D3" sqref="D3:E3"/>
+      <selection pane="topRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -587,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>18</v>
@@ -624,26 +627,8 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>23</v>
@@ -668,18 +653,6 @@
       <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
@@ -702,18 +675,6 @@
       <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="K5" s="1" t="s">
         <v>27</v>
       </c>
@@ -736,18 +697,6 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
optimization notes -- initial draft
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\UO Teaching\EDLD 654\c4-ml-fall-2021\website-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5D6F04-E3A0-498B-A168-4DC22E982C02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070AE275-3A09-4EA5-8C1C-2F1BD02F3FD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>week</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>warm-up-1</t>
+  </si>
+  <si>
+    <t>0 - precourse</t>
   </si>
 </sst>
 </file>
@@ -177,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,6 +200,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,16 +515,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I16" sqref="I16"/>
+      <selection pane="topRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.796875" style="1"/>
+    <col min="1" max="1" width="11.796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" style="1"/>
     <col min="3" max="3" width="21.69921875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.296875" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.796875" style="1"/>
@@ -536,7 +541,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -577,11 +582,8 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>44466</v>
+      <c r="A2" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -595,18 +597,6 @@
       <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
@@ -618,11 +608,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44468</v>
+      <c r="A3" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>17</v>
@@ -641,11 +628,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
+      <c r="A4" s="7">
+        <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>44473</v>
+        <v>44466</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -653,6 +640,18 @@
       <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
@@ -661,11 +660,11 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>2</v>
+      <c r="A5" s="7">
+        <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>44475</v>
+        <v>44468</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>21</v>
@@ -686,11 +685,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>3</v>
+      <c r="A6" s="7">
+        <v>2</v>
       </c>
       <c r="B6" s="2">
-        <v>44480</v>
+        <v>44473</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>22</v>
@@ -707,6 +706,12 @@
       <c r="M6" s="1" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>